<commit_message>
order placement changes for Hydroflask US
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/GoldHydroTestData1.xlsx
+++ b/src/test/resources/TestData/Hydroflask/GoldHydroTestData1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F45D1CC-C556-4C91-96EA-41AED0687A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D20E73-6B2B-4004-980D-8D1BBC129393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order_Placement" sheetId="1" r:id="rId1"/>
@@ -738,33 +738,33 @@
   <dimension ref="A1:V89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.77734375" customWidth="1"/>
-    <col min="10" max="10" width="30.5546875" customWidth="1"/>
-    <col min="11" max="11" width="19.77734375" customWidth="1"/>
-    <col min="12" max="13" width="22.21875" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="13" width="22.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.21875" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -832,7 +832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -894,7 +894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -956,7 +956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>95</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>99</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>102</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>103</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>104</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>105</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>106</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>107</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>109</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>110</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>111</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>112</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>113</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>114</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>115</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>116</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>117</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>118</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>119</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>120</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>121</v>
       </c>

</xml_diff>